<commit_message>
did some small changes
Co-Authored-By: MJ Phillip <mjphillip@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/GantChart .xlsx
+++ b/GantChart .xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristine/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristine/Documents/GitHub/2019-04-12__Procject_-Methodology-ca1_Noah-Beni/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5398922A-5CB0-ED41-A3FB-BBA4DA29CDE7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5F970C-C0E8-B944-ACAD-7832277026D6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1016,35 +1016,7 @@
     <cellStyle name="Hyperkobling" xfId="197" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="153">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FFFF"/>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FFFF"/>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
+  <dxfs count="151">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -9376,8 +9348,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="17688524" y="11294828"/>
-          <a:ext cx="3595833" cy="38100"/>
+          <a:off x="17689203" y="11426129"/>
+          <a:ext cx="3609416" cy="38100"/>
           <a:chOff x="5041200" y="3780000"/>
           <a:chExt cx="609599" cy="0"/>
         </a:xfrm>
@@ -9419,15 +9391,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>29306</xdr:colOff>
+      <xdr:colOff>149411</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>96227</xdr:rowOff>
+      <xdr:rowOff>245639</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>276956</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>134327</xdr:rowOff>
+      <xdr:colOff>3389701</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>273922</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -9442,8 +9414,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="8492124" y="10117682"/>
-          <a:ext cx="247650" cy="38100"/>
+          <a:off x="8616078" y="10380737"/>
+          <a:ext cx="3240290" cy="625930"/>
           <a:chOff x="5222175" y="3780000"/>
           <a:chExt cx="247649" cy="0"/>
         </a:xfrm>
@@ -9508,8 +9480,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm rot="10800000">
-          <a:off x="14098776" y="10157246"/>
-          <a:ext cx="2793868" cy="0"/>
+          <a:off x="14112133" y="10270889"/>
+          <a:ext cx="2784585" cy="0"/>
           <a:chOff x="5192867" y="3750693"/>
           <a:chExt cx="247649" cy="0"/>
         </a:xfrm>
@@ -9574,7 +9546,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="13408617" y="10427655"/>
+          <a:off x="13425369" y="10547184"/>
           <a:ext cx="128249" cy="162677"/>
           <a:chOff x="5212650" y="3703800"/>
           <a:chExt cx="266699" cy="152399"/>
@@ -9662,15 +9634,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>48847</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>117231</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>296497</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>155331</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -9686,7 +9658,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="11963756" y="10727504"/>
+          <a:off x="8515514" y="11447623"/>
           <a:ext cx="247650" cy="38100"/>
           <a:chOff x="5222175" y="3780000"/>
           <a:chExt cx="247649" cy="0"/>
@@ -9798,8 +9770,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="13250629" y="11905140"/>
-          <a:ext cx="998105" cy="38100"/>
+          <a:off x="13267381" y="12045270"/>
+          <a:ext cx="994710" cy="38100"/>
           <a:chOff x="5041200" y="3780000"/>
           <a:chExt cx="609599" cy="0"/>
         </a:xfrm>
@@ -9864,8 +9836,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm rot="10800000">
-          <a:off x="32399210" y="11836755"/>
-          <a:ext cx="3665105" cy="38100"/>
+          <a:off x="32396493" y="11976885"/>
+          <a:ext cx="3659220" cy="38100"/>
           <a:chOff x="5041200" y="3780000"/>
           <a:chExt cx="609599" cy="0"/>
         </a:xfrm>
@@ -9930,8 +9902,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="29309468" y="12297686"/>
-          <a:ext cx="3278777" cy="38100"/>
+          <a:off x="29302903" y="12443702"/>
+          <a:ext cx="3282625" cy="38100"/>
           <a:chOff x="5041200" y="3780000"/>
           <a:chExt cx="609599" cy="0"/>
         </a:xfrm>
@@ -9996,8 +9968,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm rot="10800000">
-          <a:off x="46575251" y="12248839"/>
-          <a:ext cx="1009652" cy="38100"/>
+          <a:off x="46625282" y="12394855"/>
+          <a:ext cx="1019612" cy="38100"/>
           <a:chOff x="5041200" y="3780000"/>
           <a:chExt cx="609599" cy="0"/>
         </a:xfrm>
@@ -10039,72 +10011,6 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>57451</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>46640</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>11199</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>160041</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="82" name="Shape 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE1D637C-BA1A-0A4B-BB43-62F124CE720B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm rot="20630230">
-          <a:off x="17687360" y="10656913"/>
-          <a:ext cx="4260203" cy="702219"/>
-          <a:chOff x="5212650" y="3703800"/>
-          <a:chExt cx="266699" cy="152399"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="83" name="Shape 14">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBCE13C8-25F2-944D-A3BA-D3762E1BE4C4}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="5212650" y="3703800"/>
-            <a:ext cx="266699" cy="152399"/>
-          </a:xfrm>
-          <a:prstGeom prst="straightConnector1">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:prstDash val="solid"/>
-            <a:round/>
-            <a:headEnd type="none" w="med" len="med"/>
-            <a:tailEnd type="none" w="med" len="med"/>
-          </a:ln>
-        </xdr:spPr>
-      </xdr:cxnSp>
-    </xdr:grpSp>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
       <xdr:colOff>29308</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>97692</xdr:rowOff>
@@ -10128,7 +10034,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="17659217" y="12866965"/>
+          <a:off x="17659896" y="13021810"/>
           <a:ext cx="247650" cy="38100"/>
           <a:chOff x="5222175" y="3780000"/>
           <a:chExt cx="247649" cy="0"/>
@@ -10841,8 +10747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:XFD156"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="80" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="P108" sqref="P108"/>
+    <sheetView tabSelected="1" zoomScale="51" zoomScaleNormal="51" zoomScaleSheetLayoutView="80" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="A97" sqref="A97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -12450,7 +12356,6 @@
         <v>43</v>
       </c>
       <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
       <c r="E33" s="7">
         <v>2</v>
       </c>
@@ -13117,27 +13022,27 @@
         <v>12</v>
       </c>
       <c r="C47" s="7">
-        <f>SUM(C4:C20)</f>
+        <f t="shared" ref="C47:H47" si="0">SUM(C4:C20)</f>
         <v>8</v>
       </c>
       <c r="D47" s="2">
-        <f>SUM(D4:D20)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="E47" s="7">
-        <f>SUM(E4:E20)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="F47" s="7">
-        <f>SUM(F4:F20)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="G47" s="7">
-        <f>SUM(G4:G20)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="H47" s="7">
-        <f>SUM(H4:H20)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="I47" s="7"/>
@@ -13146,99 +13051,99 @@
         <v>8</v>
       </c>
       <c r="K47" s="7">
-        <f>SUM(K4:K20)</f>
+        <f t="shared" ref="K47:AH47" si="1">SUM(K4:K20)</f>
         <v>10</v>
       </c>
       <c r="L47" s="7">
-        <f>SUM(L4:L20)</f>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="M47" s="7">
-        <f>SUM(M4:M20)</f>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="N47" s="7">
-        <f>SUM(N4:N20)</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="O47" s="7">
-        <f>SUM(O4:O20)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P47" s="7">
-        <f>SUM(P4:P20)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q47" s="7">
-        <f>SUM(Q4:Q20)</f>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="R47" s="7">
-        <f>SUM(R4:R20)</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="S47" s="7">
-        <f>SUM(S4:S20)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="T47" s="7">
-        <f>SUM(T4:T20)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="U47" s="7">
-        <f>SUM(U4:U20)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="V47" s="7">
-        <f>SUM(V4:V20)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W47" s="7">
-        <f>SUM(W4:W20)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="X47" s="7">
-        <f>SUM(X4:X20)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="Y47" s="7">
-        <f>SUM(Y4:Y20)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="Z47" s="7">
-        <f>SUM(Z4:Z20)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="AA47" s="7">
-        <f>SUM(AA4:AA20)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AB47" s="7">
-        <f>SUM(AB4:AB20)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC47" s="7">
-        <f>SUM(AC4:AC20)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD47" s="7">
-        <f>SUM(AD4:AD20)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE47" s="7">
-        <f>SUM(AE4:AE20)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF47" s="7">
-        <f>SUM(AF4:AF20)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AG47" s="7">
-        <f>SUM(AG4:AG20)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AH47" s="7">
-        <f>SUM(AH4:AH20)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AI47" s="8">
@@ -14303,7 +14208,7 @@
       <c r="AJ67" s="7"/>
       <c r="AK67" s="8"/>
     </row>
-    <row r="68" spans="2:37">
+    <row r="68" spans="2:37" ht="6" customHeight="1">
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
@@ -14341,7 +14246,7 @@
       <c r="AJ68" s="3"/>
       <c r="AK68" s="3"/>
     </row>
-    <row r="69" spans="2:37">
+    <row r="69" spans="2:37" hidden="1">
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
@@ -14379,7 +14284,7 @@
       <c r="AJ69" s="3"/>
       <c r="AK69" s="3"/>
     </row>
-    <row r="70" spans="2:37">
+    <row r="70" spans="2:37" hidden="1">
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
@@ -14416,7 +14321,7 @@
       <c r="AI70" s="1"/>
       <c r="AJ70" s="1"/>
     </row>
-    <row r="71" spans="2:37">
+    <row r="71" spans="2:37" hidden="1">
       <c r="B71" s="9"/>
       <c r="C71" s="9"/>
       <c r="D71" s="9"/>
@@ -14453,7 +14358,7 @@
       <c r="AI71" s="9"/>
       <c r="AJ71" s="1"/>
     </row>
-    <row r="72" spans="2:37">
+    <row r="72" spans="2:37" hidden="1">
       <c r="B72" s="9"/>
       <c r="C72" s="9"/>
       <c r="D72" s="9"/>
@@ -14490,7 +14395,7 @@
       <c r="AI72" s="9"/>
       <c r="AJ72" s="1"/>
     </row>
-    <row r="73" spans="2:37">
+    <row r="73" spans="2:37" ht="5" hidden="1">
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
@@ -14527,7 +14432,7 @@
       <c r="AI73" s="1"/>
       <c r="AJ73" s="1"/>
     </row>
-    <row r="74" spans="2:37" ht="33" customHeight="1">
+    <row r="74" spans="2:37" ht="1" hidden="1" customHeight="1">
       <c r="B74" s="86" t="s">
         <v>63</v>
       </c>
@@ -14566,7 +14471,7 @@
       <c r="AI74" s="10"/>
       <c r="AJ74" s="1"/>
     </row>
-    <row r="75" spans="2:37" ht="38" customHeight="1">
+    <row r="75" spans="2:37" ht="1" hidden="1" customHeight="1">
       <c r="B75" s="84">
         <v>30</v>
       </c>
@@ -14605,7 +14510,7 @@
       <c r="AI75" s="3"/>
       <c r="AJ75" s="1"/>
     </row>
-    <row r="76" spans="2:37" ht="19">
+    <row r="76" spans="2:37" ht="19" hidden="1">
       <c r="B76" s="84">
         <v>28</v>
       </c>
@@ -14644,7 +14549,7 @@
       <c r="AI76" s="4"/>
       <c r="AJ76" s="1"/>
     </row>
-    <row r="77" spans="2:37" ht="19">
+    <row r="77" spans="2:37" ht="19" hidden="1">
       <c r="B77" s="84">
         <v>28</v>
       </c>
@@ -14683,7 +14588,7 @@
       <c r="AI77" s="4"/>
       <c r="AJ77" s="1"/>
     </row>
-    <row r="78" spans="2:37" ht="19">
+    <row r="78" spans="2:37" ht="1" hidden="1">
       <c r="B78" s="84">
         <v>27</v>
       </c>
@@ -14722,7 +14627,7 @@
       <c r="AI78" s="4"/>
       <c r="AJ78" s="1"/>
     </row>
-    <row r="79" spans="2:37" ht="19">
+    <row r="79" spans="2:37" ht="1" hidden="1">
       <c r="B79" s="84">
         <v>26</v>
       </c>
@@ -14761,7 +14666,7 @@
       <c r="AI79" s="4"/>
       <c r="AJ79" s="1"/>
     </row>
-    <row r="80" spans="2:37" ht="19">
+    <row r="80" spans="2:37" ht="205" customHeight="1">
       <c r="B80" s="84">
         <v>25</v>
       </c>
@@ -15232,7 +15137,7 @@
       <c r="AI91" s="3"/>
       <c r="AJ91" s="9"/>
     </row>
-    <row r="92" spans="1:36" s="2" customFormat="1" ht="19">
+    <row r="92" spans="1:36" s="2" customFormat="1" ht="80" customHeight="1">
       <c r="B92" s="85">
         <v>13</v>
       </c>
@@ -15432,7 +15337,7 @@
       <c r="AI96" s="3"/>
       <c r="AJ96" s="1"/>
     </row>
-    <row r="97" spans="1:37" ht="37" customHeight="1">
+    <row r="97" spans="1:37" ht="100" customHeight="1">
       <c r="B97" s="83">
         <v>8</v>
       </c>
@@ -15478,7 +15383,7 @@
       <c r="AJ97" s="10"/>
       <c r="AK97" s="8"/>
     </row>
-    <row r="98" spans="1:37" ht="44" customHeight="1">
+    <row r="98" spans="1:37" ht="85" customHeight="1">
       <c r="B98" s="83">
         <v>7</v>
       </c>
@@ -15526,7 +15431,7 @@
       <c r="AJ98" s="3"/>
       <c r="AK98" s="3"/>
     </row>
-    <row r="99" spans="1:37" ht="38" customHeight="1">
+    <row r="99" spans="1:37" ht="91" customHeight="1">
       <c r="B99" s="83">
         <v>6</v>
       </c>
@@ -17293,757 +17198,757 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G76:J82 D11:AI11 C76:F79 AJ51:AJ58 K76:AI83 AJ99:AJ106 C8 C10 D8:D10 C5:O5 K12:V12 Q5:AB5 E10:AB10 X12:AB12 C4:AB4 C6:AB7 AE12:AH12 AE4:AH10 C12:H12 F8:AB9 T124:AI131 N119:P126 E119:H122 I119:M123 C81:F83 D80:F80">
-    <cfRule type="cellIs" dxfId="152" priority="159" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="150" priority="159" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA95:AH98 C48:AH51 Y133:AD133 V135:AE135 AJ59:AJ66 C84:AI91 AJ68:AJ69 C93:AI94 AJ111 AG136:AI136 C13 E13:U13 C52:F52 C17:AH17 O14:U16 R18:U19 S21:U21 C18:P23 C24:X24 C25:Y25 C26:Z26 C27:AA27 AB26:AH26 AA23:AH25 Z22:AH22 Y21:AH21 X18:AH20 X13:AH16 I28 O28:P28 V28:W28 AC27:AH27 AC28:AD28 C31 E31:AH31 C30:AH30 D12:H12 C14:K16 C29:AG29 V43:W46 AC43:AD46 C32:AH42 O43:P46 I43:I45 H52:O52 C53:O53 Q52:AH53 C133:M138 C124:M131 C98:E98 C97 E97 C95:E95 G95:Z95 O98:Z98 M96:Z97 C96:K96 G97:G98 I97:K97 I98 K98:M98">
-    <cfRule type="cellIs" dxfId="151" priority="160" stopIfTrue="1" operator="greaterThan">
+  <conditionalFormatting sqref="AA95:AH98 C48:AH51 Y133:AD133 V135:AE135 AJ59:AJ66 C84:AI91 AJ68:AJ69 C93:AI94 AJ111 AG136:AI136 C13 E13:U13 C52:F52 C17:AH17 O14:U16 R18:U19 S21:U21 C18:P23 C24:X24 C25:Y25 C26:Z26 C27:AA27 AB26:AH26 AA23:AH25 Z22:AH22 Y21:AH21 X18:AH20 X13:AH16 I28 O28:P28 V28:W28 AC27:AH27 AC28:AD28 C31 E31:AH31 C30:AH30 D12:H12 C14:K16 C29:AG29 V43:W46 AC43:AD46 O43:P46 I43:I45 H52:O52 C53:O53 Q52:AH53 C133:M138 C124:M131 C98:E98 C97 E97 C95:E95 G95:Z95 O98:Z98 M96:Z97 C96:K96 G97:G98 I97:K97 I98 K98:M98 C32:AH32 C33 E33:AH33 C34:AH42">
+    <cfRule type="cellIs" dxfId="149" priority="160" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12:J12">
-    <cfRule type="cellIs" dxfId="150" priority="162" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="148" priority="162" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G83:J83">
-    <cfRule type="cellIs" dxfId="149" priority="163" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="147" priority="163" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V132:W132">
-    <cfRule type="cellIs" dxfId="148" priority="167" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="146" priority="167" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA137:AB137">
-    <cfRule type="cellIs" dxfId="147" priority="169" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="145" priority="169" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G52">
-    <cfRule type="cellIs" dxfId="146" priority="158" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="144" priority="158" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L14">
-    <cfRule type="cellIs" dxfId="145" priority="157" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="143" priority="157" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M14">
-    <cfRule type="cellIs" dxfId="144" priority="156" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="142" priority="156" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N14">
-    <cfRule type="cellIs" dxfId="143" priority="155" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="141" priority="155" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L15">
-    <cfRule type="cellIs" dxfId="142" priority="154" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="140" priority="154" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M15">
-    <cfRule type="cellIs" dxfId="141" priority="153" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="139" priority="153" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N15">
-    <cfRule type="cellIs" dxfId="140" priority="152" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="138" priority="152" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L16">
-    <cfRule type="cellIs" dxfId="139" priority="151" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="137" priority="151" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M16">
-    <cfRule type="cellIs" dxfId="138" priority="150" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="136" priority="150" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N16">
-    <cfRule type="cellIs" dxfId="137" priority="149" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="135" priority="149" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P5">
-    <cfRule type="cellIs" dxfId="136" priority="148" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="134" priority="148" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V13">
-    <cfRule type="cellIs" dxfId="135" priority="147" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="133" priority="147" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V14">
-    <cfRule type="cellIs" dxfId="134" priority="146" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="132" priority="146" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V15">
-    <cfRule type="cellIs" dxfId="133" priority="145" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="131" priority="145" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V16">
-    <cfRule type="cellIs" dxfId="132" priority="144" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="130" priority="144" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V18">
-    <cfRule type="cellIs" dxfId="131" priority="143" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="129" priority="143" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V19">
-    <cfRule type="cellIs" dxfId="130" priority="142" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="128" priority="142" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V20:V21">
-    <cfRule type="cellIs" dxfId="129" priority="140" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="127" priority="140" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W12:W16">
-    <cfRule type="cellIs" dxfId="128" priority="137" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="126" priority="137" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W18:W23">
-    <cfRule type="cellIs" dxfId="127" priority="136" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="125" priority="136" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q18">
-    <cfRule type="cellIs" dxfId="126" priority="134" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="124" priority="134" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V22">
-    <cfRule type="cellIs" dxfId="125" priority="132" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="123" priority="132" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V23">
-    <cfRule type="cellIs" dxfId="124" priority="131" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="122" priority="131" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD8">
-    <cfRule type="cellIs" dxfId="123" priority="116" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="121" priority="116" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC5">
-    <cfRule type="cellIs" dxfId="122" priority="129" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="120" priority="129" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC6">
-    <cfRule type="cellIs" dxfId="121" priority="128" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="119" priority="128" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC7">
-    <cfRule type="cellIs" dxfId="120" priority="127" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="118" priority="127" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC12">
-    <cfRule type="cellIs" dxfId="119" priority="126" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="117" priority="126" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC10">
-    <cfRule type="cellIs" dxfId="118" priority="125" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="116" priority="125" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC9">
-    <cfRule type="cellIs" dxfId="117" priority="124" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="115" priority="124" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC8">
-    <cfRule type="cellIs" dxfId="116" priority="123" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="114" priority="123" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD4">
-    <cfRule type="cellIs" dxfId="115" priority="122" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="113" priority="122" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD5">
-    <cfRule type="cellIs" dxfId="114" priority="121" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="112" priority="121" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD6">
-    <cfRule type="cellIs" dxfId="113" priority="120" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="111" priority="120" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD12">
-    <cfRule type="cellIs" dxfId="112" priority="119" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="110" priority="119" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD10">
-    <cfRule type="cellIs" dxfId="111" priority="118" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="109" priority="118" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD9">
-    <cfRule type="cellIs" dxfId="110" priority="117" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="108" priority="117" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31">
-    <cfRule type="cellIs" dxfId="109" priority="115" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="107" priority="115" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC4">
-    <cfRule type="cellIs" dxfId="108" priority="114" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="106" priority="114" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I46">
-    <cfRule type="cellIs" dxfId="107" priority="113" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="105" priority="113" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D54">
-    <cfRule type="cellIs" dxfId="106" priority="112" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="104" priority="112" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55">
-    <cfRule type="cellIs" dxfId="105" priority="78" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="103" priority="78" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="cellIs" dxfId="104" priority="110" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="102" priority="110" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E54">
-    <cfRule type="cellIs" dxfId="103" priority="109" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="101" priority="109" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F54">
-    <cfRule type="cellIs" dxfId="102" priority="108" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="100" priority="108" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G54">
-    <cfRule type="cellIs" dxfId="101" priority="107" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="99" priority="107" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H54">
-    <cfRule type="cellIs" dxfId="100" priority="106" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="98" priority="106" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I54">
-    <cfRule type="cellIs" dxfId="99" priority="105" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="97" priority="105" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J54">
-    <cfRule type="cellIs" dxfId="98" priority="104" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="96" priority="104" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K54">
-    <cfRule type="cellIs" dxfId="97" priority="103" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="95" priority="103" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L54">
-    <cfRule type="cellIs" dxfId="96" priority="102" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="94" priority="102" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M54">
-    <cfRule type="cellIs" dxfId="95" priority="101" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="93" priority="101" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N54">
-    <cfRule type="cellIs" dxfId="94" priority="100" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="92" priority="100" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O54">
-    <cfRule type="cellIs" dxfId="93" priority="99" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="91" priority="99" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q54">
-    <cfRule type="cellIs" dxfId="92" priority="98" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="90" priority="98" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R54">
-    <cfRule type="cellIs" dxfId="91" priority="97" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="89" priority="97" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S54">
-    <cfRule type="cellIs" dxfId="90" priority="96" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="88" priority="96" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T54">
-    <cfRule type="cellIs" dxfId="89" priority="95" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="87" priority="95" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U54">
-    <cfRule type="cellIs" dxfId="88" priority="94" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="86" priority="94" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V54">
-    <cfRule type="cellIs" dxfId="87" priority="93" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="85" priority="93" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W54">
-    <cfRule type="cellIs" dxfId="86" priority="92" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="84" priority="92" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X54">
-    <cfRule type="cellIs" dxfId="85" priority="91" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="83" priority="91" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y54">
-    <cfRule type="cellIs" dxfId="84" priority="90" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="82" priority="90" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z54">
-    <cfRule type="cellIs" dxfId="83" priority="89" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="81" priority="89" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA57">
-    <cfRule type="cellIs" dxfId="82" priority="8" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="80" priority="8" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="XFD54">
-    <cfRule type="cellIs" dxfId="81" priority="87" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="79" priority="87" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA54">
-    <cfRule type="cellIs" dxfId="80" priority="86" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="78" priority="86" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB54">
-    <cfRule type="cellIs" dxfId="79" priority="85" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="77" priority="85" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD54">
-    <cfRule type="cellIs" dxfId="78" priority="84" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="76" priority="84" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55">
-    <cfRule type="cellIs" dxfId="77" priority="83" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="75" priority="83" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D55">
-    <cfRule type="cellIs" dxfId="76" priority="82" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="74" priority="82" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E55">
-    <cfRule type="cellIs" dxfId="75" priority="81" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="73" priority="81" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F55">
-    <cfRule type="cellIs" dxfId="74" priority="80" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="72" priority="80" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G55">
-    <cfRule type="cellIs" dxfId="73" priority="79" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="71" priority="79" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I55">
-    <cfRule type="cellIs" dxfId="72" priority="77" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="70" priority="77" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J55">
-    <cfRule type="cellIs" dxfId="71" priority="76" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="69" priority="76" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K55">
-    <cfRule type="cellIs" dxfId="70" priority="75" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="68" priority="75" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L55">
-    <cfRule type="cellIs" dxfId="69" priority="74" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="67" priority="74" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M55">
-    <cfRule type="cellIs" dxfId="68" priority="73" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="66" priority="73" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N55">
-    <cfRule type="cellIs" dxfId="67" priority="72" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="65" priority="72" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O55">
-    <cfRule type="cellIs" dxfId="66" priority="71" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="64" priority="71" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q55">
-    <cfRule type="cellIs" dxfId="65" priority="70" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="63" priority="70" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R55">
-    <cfRule type="cellIs" dxfId="64" priority="69" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="62" priority="69" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S55">
-    <cfRule type="cellIs" dxfId="63" priority="68" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="61" priority="68" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T55">
-    <cfRule type="cellIs" dxfId="62" priority="67" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="60" priority="67" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U55">
-    <cfRule type="cellIs" dxfId="61" priority="66" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="59" priority="66" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V55">
-    <cfRule type="cellIs" dxfId="60" priority="65" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="58" priority="65" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W55">
-    <cfRule type="cellIs" dxfId="59" priority="64" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="57" priority="64" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X55">
-    <cfRule type="cellIs" dxfId="58" priority="63" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="56" priority="63" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y55">
-    <cfRule type="cellIs" dxfId="57" priority="62" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="55" priority="62" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA55">
-    <cfRule type="cellIs" dxfId="56" priority="61" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="54" priority="61" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z55">
-    <cfRule type="cellIs" dxfId="55" priority="60" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="53" priority="60" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB55">
-    <cfRule type="cellIs" dxfId="54" priority="59" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="52" priority="59" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56">
-    <cfRule type="cellIs" dxfId="53" priority="58" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="51" priority="58" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D56">
-    <cfRule type="cellIs" dxfId="52" priority="57" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="50" priority="57" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E56">
-    <cfRule type="cellIs" dxfId="51" priority="56" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="49" priority="56" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F56">
-    <cfRule type="cellIs" dxfId="50" priority="55" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="48" priority="55" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G56">
-    <cfRule type="cellIs" dxfId="49" priority="54" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="47" priority="54" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H56">
-    <cfRule type="cellIs" dxfId="48" priority="53" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="46" priority="53" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I56">
-    <cfRule type="cellIs" dxfId="47" priority="52" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="45" priority="52" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J56">
-    <cfRule type="cellIs" dxfId="46" priority="51" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="44" priority="51" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K56">
-    <cfRule type="cellIs" dxfId="45" priority="50" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="43" priority="50" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q56">
-    <cfRule type="cellIs" dxfId="44" priority="49" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="42" priority="49" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R56">
-    <cfRule type="cellIs" dxfId="43" priority="48" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="41" priority="48" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S56">
-    <cfRule type="cellIs" dxfId="42" priority="47" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="40" priority="47" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T56">
-    <cfRule type="cellIs" dxfId="41" priority="46" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="46" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U56">
-    <cfRule type="cellIs" dxfId="40" priority="45" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="38" priority="45" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V56">
-    <cfRule type="cellIs" dxfId="39" priority="44" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="37" priority="44" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D57">
-    <cfRule type="cellIs" dxfId="38" priority="37" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="36" priority="37" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X56">
-    <cfRule type="cellIs" dxfId="37" priority="42" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="42" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y56">
-    <cfRule type="cellIs" dxfId="36" priority="41" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="34" priority="41" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z56">
-    <cfRule type="cellIs" dxfId="35" priority="40" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="40" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA56">
-    <cfRule type="cellIs" dxfId="34" priority="39" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="32" priority="39" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57">
-    <cfRule type="cellIs" dxfId="33" priority="38" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="38" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G57">
-    <cfRule type="cellIs" dxfId="32" priority="34" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="34" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E57">
-    <cfRule type="cellIs" dxfId="31" priority="36" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="36" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57">
-    <cfRule type="cellIs" dxfId="30" priority="35" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="28" priority="35" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H57">
-    <cfRule type="cellIs" dxfId="29" priority="33" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="33" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I57">
-    <cfRule type="cellIs" dxfId="28" priority="32" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="32" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J57">
-    <cfRule type="cellIs" dxfId="27" priority="31" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="31" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K57">
-    <cfRule type="cellIs" dxfId="26" priority="30" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="30" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L57">
-    <cfRule type="cellIs" dxfId="25" priority="29" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="29" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L56">
-    <cfRule type="cellIs" dxfId="24" priority="28" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="28" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M56">
-    <cfRule type="cellIs" dxfId="23" priority="27" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="27" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M57">
-    <cfRule type="cellIs" dxfId="22" priority="26" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="26" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N57">
-    <cfRule type="cellIs" dxfId="21" priority="25" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="25" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N56">
-    <cfRule type="cellIs" dxfId="20" priority="24" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="24" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O56">
-    <cfRule type="cellIs" dxfId="19" priority="23" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="23" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O57">
-    <cfRule type="cellIs" dxfId="18" priority="22" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="22" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P57">
-    <cfRule type="cellIs" dxfId="17" priority="21" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="21" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P56">
-    <cfRule type="cellIs" dxfId="16" priority="20" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="20" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q57">
-    <cfRule type="cellIs" dxfId="15" priority="19" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="19" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R57">
-    <cfRule type="cellIs" dxfId="14" priority="18" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="18" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S57">
-    <cfRule type="cellIs" dxfId="13" priority="17" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="17" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T57">
-    <cfRule type="cellIs" dxfId="12" priority="16" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="16" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U57">
-    <cfRule type="cellIs" dxfId="11" priority="15" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="15" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V57">
-    <cfRule type="cellIs" dxfId="10" priority="14" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="14" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W56">
-    <cfRule type="cellIs" dxfId="9" priority="13" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="13" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W57">
-    <cfRule type="cellIs" dxfId="8" priority="12" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="12" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X57">
-    <cfRule type="cellIs" dxfId="7" priority="11" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="11" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y57">
-    <cfRule type="cellIs" dxfId="6" priority="10" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="10" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z57">
-    <cfRule type="cellIs" dxfId="5" priority="9" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="9" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E123:H123">
-    <cfRule type="cellIs" dxfId="4" priority="7" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="7" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F95">
-    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="3" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F100">
-    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>